<commit_message>
tradotto in inglese dispensa test 2 campioni
</commit_message>
<xml_diff>
--- a/sequenza lezioni BDA.xlsx
+++ b/sequenza lezioni BDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/my bda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD12207-7A89-A84E-8F78-7BEC81714A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8DEC3F-AA89-814D-990F-4182263A3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,7 +242,7 @@
     <t>ripresa MCMC, prob programming inclusa ROPE</t>
   </si>
   <si>
-    <t>Notebook normal-normal; assignment negli ultimi 20 min</t>
+    <t>Notebook normal-normal; assignment negli ultimi 20 min (chiedere se data ok)</t>
   </si>
 </sst>
 </file>
@@ -855,7 +855,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E5" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated normal-normal, discussing qtiles of normal and t
</commit_message>
<xml_diff>
--- a/sequenza lezioni BDA.xlsx
+++ b/sequenza lezioni BDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/my bda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8DEC3F-AA89-814D-990F-4182263A3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63333EC-35A2-F54A-90CC-8B626BFF4AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Previsione</t>
   </si>
@@ -854,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -1324,6 +1324,9 @@
         <f t="shared" si="9"/>
         <v>45596</v>
       </c>
+      <c r="H19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1350,6 +1353,9 @@
       <c r="G20" s="14">
         <f t="shared" si="9"/>
         <v>45600</v>
+      </c>
+      <c r="H20" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>